<commit_message>
ultimo cambio de configuración a la pantalla
</commit_message>
<xml_diff>
--- a/resources/fraudes.xlsx
+++ b/resources/fraudes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AC6579-0DF1-427D-947B-3E64ADDE04BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782C60FC-5B49-4C9A-8C8B-D8AACB267FCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" xr2:uid="{3A9A6D73-6191-460D-924B-586DA52215C8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>REFERENCIAS:</t>
   </si>
@@ -33,49 +33,403 @@
     <t>FECHA:</t>
   </si>
   <si>
-    <t>42691263074200660192711</t>
-  </si>
-  <si>
-    <t>42691263074200660192601</t>
-  </si>
-  <si>
     <t>42691263074200660192611</t>
   </si>
   <si>
-    <t>42691263074200660192621</t>
-  </si>
-  <si>
-    <t>42691263074200660192631</t>
-  </si>
-  <si>
-    <t>42691263074200660192641</t>
-  </si>
-  <si>
-    <t>42691263074200660192651</t>
-  </si>
-  <si>
-    <t>42691263074200660192661</t>
-  </si>
-  <si>
-    <t>42691263074200660192671</t>
-  </si>
-  <si>
-    <t>42691263074200660192681</t>
-  </si>
-  <si>
-    <t>42691263074200660192691</t>
-  </si>
-  <si>
     <t>42691263074200660192701</t>
   </si>
   <si>
-    <t>42691263074200660192721</t>
-  </si>
-  <si>
-    <t>42691263074200660192731</t>
-  </si>
-  <si>
-    <t>42691263074200660192741</t>
+    <t>42691263074200660191061</t>
+  </si>
+  <si>
+    <t>42691263074200660191072</t>
+  </si>
+  <si>
+    <t>42691263074200660191083</t>
+  </si>
+  <si>
+    <t>42691263074200660191094</t>
+  </si>
+  <si>
+    <t>42691263074200660191105</t>
+  </si>
+  <si>
+    <t>42691263074200660191116</t>
+  </si>
+  <si>
+    <t>42691263074200660191127</t>
+  </si>
+  <si>
+    <t>42691263074200660191138</t>
+  </si>
+  <si>
+    <t>42691263074200660191149</t>
+  </si>
+  <si>
+    <t>42691263074200660191151</t>
+  </si>
+  <si>
+    <t>42691263074200660191162</t>
+  </si>
+  <si>
+    <t>42691263074200660191173</t>
+  </si>
+  <si>
+    <t>42691263074200660191184</t>
+  </si>
+  <si>
+    <t>42691263074200660191195</t>
+  </si>
+  <si>
+    <t>42691263074200660191206</t>
+  </si>
+  <si>
+    <t>42691263074200660191217</t>
+  </si>
+  <si>
+    <t>42691263074200660191228</t>
+  </si>
+  <si>
+    <t>42691263074200660191239</t>
+  </si>
+  <si>
+    <t>42691263074200660191241</t>
+  </si>
+  <si>
+    <t>42691263074200660191252</t>
+  </si>
+  <si>
+    <t>42691263074200660191263</t>
+  </si>
+  <si>
+    <t>42691263074200660191274</t>
+  </si>
+  <si>
+    <t>42691263074200660191285</t>
+  </si>
+  <si>
+    <t>42691263074200660191296</t>
+  </si>
+  <si>
+    <t>42691263074200660191307</t>
+  </si>
+  <si>
+    <t>42691263074200660192101</t>
+  </si>
+  <si>
+    <t>42691263074200660192102</t>
+  </si>
+  <si>
+    <t>42691263074200660192103</t>
+  </si>
+  <si>
+    <t>42691263074200660192104</t>
+  </si>
+  <si>
+    <t>42691263074200660192105</t>
+  </si>
+  <si>
+    <t>42691263074200660192106</t>
+  </si>
+  <si>
+    <t>42691263074200660192107</t>
+  </si>
+  <si>
+    <t>42691263074200660192108</t>
+  </si>
+  <si>
+    <t>42691263074200660192109</t>
+  </si>
+  <si>
+    <t>42691263074200660192111</t>
+  </si>
+  <si>
+    <t>42691263074200660192122</t>
+  </si>
+  <si>
+    <t>42691263074200660192133</t>
+  </si>
+  <si>
+    <t>42691263074200660192444</t>
+  </si>
+  <si>
+    <t>42691263074200660192115</t>
+  </si>
+  <si>
+    <t>42691263074200660192126</t>
+  </si>
+  <si>
+    <t>42691263074200660192137</t>
+  </si>
+  <si>
+    <t>42691263074200660192148</t>
+  </si>
+  <si>
+    <t>42691263074200660192159</t>
+  </si>
+  <si>
+    <t>42691263074200660192161</t>
+  </si>
+  <si>
+    <t>42691263074200660192172</t>
+  </si>
+  <si>
+    <t>42691263074200660192183</t>
+  </si>
+  <si>
+    <t>42691263074200660192194</t>
+  </si>
+  <si>
+    <t>42691263074200660192205</t>
+  </si>
+  <si>
+    <t>42691263074200660192216</t>
+  </si>
+  <si>
+    <t>42691263074200660192227</t>
+  </si>
+  <si>
+    <t>42691263074200660192238</t>
+  </si>
+  <si>
+    <t>42691263074200660192249</t>
+  </si>
+  <si>
+    <t>42691263074200660192251</t>
+  </si>
+  <si>
+    <t>42691263074200660192262</t>
+  </si>
+  <si>
+    <t>42691263074200660192273</t>
+  </si>
+  <si>
+    <t>42691263074200660192284</t>
+  </si>
+  <si>
+    <t>42691263074200660192295</t>
+  </si>
+  <si>
+    <t>42691263074200660192306</t>
+  </si>
+  <si>
+    <t>42691263074200660192317</t>
+  </si>
+  <si>
+    <t>42691263074200660192328</t>
+  </si>
+  <si>
+    <t>42691263074200660192339</t>
+  </si>
+  <si>
+    <t>42691263074200660192341</t>
+  </si>
+  <si>
+    <t>42691263074200660192352</t>
+  </si>
+  <si>
+    <t>42691263074200660192363</t>
+  </si>
+  <si>
+    <t>42691263074200660192374</t>
+  </si>
+  <si>
+    <t>42691263074200660192385</t>
+  </si>
+  <si>
+    <t>42691263074200660192396</t>
+  </si>
+  <si>
+    <t>42691263074200660192407</t>
+  </si>
+  <si>
+    <t>42691263074200660192418</t>
+  </si>
+  <si>
+    <t>42691263074200660192429</t>
+  </si>
+  <si>
+    <t>42691263074200660192431</t>
+  </si>
+  <si>
+    <t>42691263074200660192442</t>
+  </si>
+  <si>
+    <t>42691263074200660192453</t>
+  </si>
+  <si>
+    <t>42691263074200660192464</t>
+  </si>
+  <si>
+    <t>42691263074200660192475</t>
+  </si>
+  <si>
+    <t>42691263074200660192486</t>
+  </si>
+  <si>
+    <t>42691263074200660192497</t>
+  </si>
+  <si>
+    <t>42691263074200660192508</t>
+  </si>
+  <si>
+    <t>42691263074200660192519</t>
+  </si>
+  <si>
+    <t>42691263074200660192521</t>
+  </si>
+  <si>
+    <t>42691263074200660192532</t>
+  </si>
+  <si>
+    <t>42691263074200660192543</t>
+  </si>
+  <si>
+    <t>42691263074200660192554</t>
+  </si>
+  <si>
+    <t>42691263074200660192565</t>
+  </si>
+  <si>
+    <t>42691263074200660192576</t>
+  </si>
+  <si>
+    <t>42691263074200660192587</t>
+  </si>
+  <si>
+    <t>42691263074200660192598</t>
+  </si>
+  <si>
+    <t>42691263074200660192609</t>
+  </si>
+  <si>
+    <t>42691263074200660192622</t>
+  </si>
+  <si>
+    <t>42691263074200660192633</t>
+  </si>
+  <si>
+    <t>42691263074200660192644</t>
+  </si>
+  <si>
+    <t>42691263074200660192655</t>
+  </si>
+  <si>
+    <t>42691263074200660192666</t>
+  </si>
+  <si>
+    <t>42691263074200660192677</t>
+  </si>
+  <si>
+    <t>42691263074200660192688</t>
+  </si>
+  <si>
+    <t>42691263074200660192699</t>
+  </si>
+  <si>
+    <t>42691263074200660192712</t>
+  </si>
+  <si>
+    <t>42691263074200660192723</t>
+  </si>
+  <si>
+    <t>42691263074200660192734</t>
+  </si>
+  <si>
+    <t>42691263074200660192745</t>
+  </si>
+  <si>
+    <t>42691263074200660192756</t>
+  </si>
+  <si>
+    <t>42691263074200660192767</t>
+  </si>
+  <si>
+    <t>42691263074200660192778</t>
+  </si>
+  <si>
+    <t>42691263074200660192789</t>
+  </si>
+  <si>
+    <t>42691263074200660192791</t>
+  </si>
+  <si>
+    <t>42691263074200660192802</t>
+  </si>
+  <si>
+    <t>42691263074200660192813</t>
+  </si>
+  <si>
+    <t>42691263074200660192824</t>
+  </si>
+  <si>
+    <t>42691263074200660192835</t>
+  </si>
+  <si>
+    <t>42691263074200660192846</t>
+  </si>
+  <si>
+    <t>42691263074200660192857</t>
+  </si>
+  <si>
+    <t>42691263074200660192868</t>
+  </si>
+  <si>
+    <t>42691263074200660192879</t>
+  </si>
+  <si>
+    <t>42691263074200660192881</t>
+  </si>
+  <si>
+    <t>42691263074200660192892</t>
+  </si>
+  <si>
+    <t>42691263074200660192903</t>
+  </si>
+  <si>
+    <t>42691263074200660192914</t>
+  </si>
+  <si>
+    <t>42691263074200660192925</t>
+  </si>
+  <si>
+    <t>42691263074200660192936</t>
+  </si>
+  <si>
+    <t>42691263074200660192947</t>
+  </si>
+  <si>
+    <t>42691263074200660192958</t>
+  </si>
+  <si>
+    <t>42691263074200660192969</t>
+  </si>
+  <si>
+    <t>42691263074200660192971</t>
+  </si>
+  <si>
+    <t>42691263074200660192982</t>
+  </si>
+  <si>
+    <t>42691263074200660192993</t>
+  </si>
+  <si>
+    <t>42691263074200660191004</t>
+  </si>
+  <si>
+    <t>42691263074200660191015</t>
+  </si>
+  <si>
+    <t>42691263074200660191026</t>
+  </si>
+  <si>
+    <t>42691263074200660191037</t>
+  </si>
+  <si>
+    <t>42691263074200660191048</t>
+  </si>
+  <si>
+    <t>42691263074200660191059</t>
   </si>
 </sst>
 </file>
@@ -91,18 +445,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,7 +468,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F36BCC6-92E4-483A-A6E0-F70FDCFF8E32}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,7 +805,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1">
         <v>45484</v>
@@ -465,72 +813,662 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>